<commit_message>
SEM 5 - 28/11/2023
</commit_message>
<xml_diff>
--- a/SEM 5/STE/Documentation/STEEXP1.xlsx
+++ b/SEM 5/STE/Documentation/STEEXP1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6434322-49A8-4A21-AA22-41D243E14126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F64BB0-0B06-439F-8F00-40F1CB9186FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,9 +543,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -583,9 +583,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,9 +618,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,9 +670,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -832,20 +866,25 @@
   <dimension ref="B1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="1" customWidth="1"/>
-    <col min="4" max="9" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -871,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
@@ -897,7 +936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -923,7 +962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
@@ -949,7 +988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
@@ -975,7 +1014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
@@ -1001,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>24</v>
       </c>

</xml_diff>